<commit_message>
add nla hw12 all
</commit_message>
<xml_diff>
--- a/MTH9821/HW12_submit.xlsx
+++ b/MTH9821/HW12_submit.xlsx
@@ -1457,7 +1457,7 @@
   <sheetPr/>
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>
@@ -1598,7 +1598,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="13.2"/>
@@ -1679,13 +1679,27 @@
       <c r="B5" s="23">
         <v>200</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
+      <c r="C5" s="24">
+        <v>50</v>
+      </c>
+      <c r="D5" s="24">
+        <v>4.28080088503871</v>
+      </c>
+      <c r="E5" s="24">
+        <v>0.0947987669223922</v>
+      </c>
+      <c r="F5" s="24">
+        <v>16</v>
+      </c>
+      <c r="G5" s="24">
+        <v>625</v>
+      </c>
+      <c r="H5" s="24">
+        <v>4.40888133315568</v>
+      </c>
+      <c r="I5" s="24">
+        <v>0.0332816811945804</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="22">
@@ -1694,13 +1708,27 @@
       <c r="B6" s="23">
         <v>200</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
+      <c r="C6" s="24">
+        <v>100</v>
+      </c>
+      <c r="D6" s="24">
+        <v>4.58657835828742</v>
+      </c>
+      <c r="E6" s="24">
+        <v>0.210978706326314</v>
+      </c>
+      <c r="F6" s="24">
+        <v>19</v>
+      </c>
+      <c r="G6" s="24">
+        <v>1052</v>
+      </c>
+      <c r="H6" s="24">
+        <v>4.62500251244694</v>
+      </c>
+      <c r="I6" s="24">
+        <v>0.249402860485834</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="22">
@@ -1709,13 +1737,27 @@
       <c r="B7" s="23">
         <v>200</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
+      <c r="C7" s="24">
+        <v>200</v>
+      </c>
+      <c r="D7" s="24">
+        <v>4.39805070067437</v>
+      </c>
+      <c r="E7" s="24">
+        <v>0.0224510487132709</v>
+      </c>
+      <c r="F7" s="24">
+        <v>24</v>
+      </c>
+      <c r="G7" s="24">
+        <v>1666</v>
+      </c>
+      <c r="H7" s="24">
+        <v>4.66672508017509</v>
+      </c>
+      <c r="I7" s="24">
+        <v>0.291125428213986</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="22">
@@ -1724,13 +1766,27 @@
       <c r="B8" s="23">
         <v>200</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
+      <c r="C8" s="24">
+        <v>400</v>
+      </c>
+      <c r="D8" s="24">
+        <v>4.34792558663446</v>
+      </c>
+      <c r="E8" s="24">
+        <v>0.0276740653266438</v>
+      </c>
+      <c r="F8" s="24">
+        <v>31</v>
+      </c>
+      <c r="G8" s="24">
+        <v>2580</v>
+      </c>
+      <c r="H8" s="24">
+        <v>4.57791452407996</v>
+      </c>
+      <c r="I8" s="24">
+        <v>0.202314872118854</v>
+      </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="22">
@@ -1739,13 +1795,27 @@
       <c r="B9" s="23">
         <v>200</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
+      <c r="C9" s="24">
+        <v>800</v>
+      </c>
+      <c r="D9" s="24">
+        <v>4.25059304136649</v>
+      </c>
+      <c r="E9" s="24">
+        <v>0.125006610594615</v>
+      </c>
+      <c r="F9" s="24">
+        <v>38</v>
+      </c>
+      <c r="G9" s="24">
+        <v>4210</v>
+      </c>
+      <c r="H9" s="24">
+        <v>4.54837295748209</v>
+      </c>
+      <c r="I9" s="24">
+        <v>0.172773305520983</v>
+      </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="22">
@@ -1754,13 +1824,27 @@
       <c r="B10" s="23">
         <v>200</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
+      <c r="C10" s="24">
+        <v>1600</v>
+      </c>
+      <c r="D10" s="24">
+        <v>4.36051467974151</v>
+      </c>
+      <c r="E10" s="24">
+        <v>0.0150849722195909</v>
+      </c>
+      <c r="F10" s="24">
+        <v>48</v>
+      </c>
+      <c r="G10" s="24">
+        <v>6666</v>
+      </c>
+      <c r="H10" s="24">
+        <v>4.56041966834008</v>
+      </c>
+      <c r="I10" s="24">
+        <v>0.184820016378974</v>
+      </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="22">
@@ -1769,13 +1853,27 @@
       <c r="B11" s="23">
         <v>200</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
+      <c r="C11" s="24">
+        <v>3200</v>
+      </c>
+      <c r="D11" s="24">
+        <v>4.4807543434916</v>
+      </c>
+      <c r="E11" s="24">
+        <v>0.105154691530498</v>
+      </c>
+      <c r="F11" s="24">
+        <v>61</v>
+      </c>
+      <c r="G11" s="24">
+        <v>10491</v>
+      </c>
+      <c r="H11" s="24">
+        <v>4.55986997428762</v>
+      </c>
+      <c r="I11" s="24">
+        <v>0.184270322326512</v>
+      </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="22">
@@ -1784,13 +1882,27 @@
       <c r="B12" s="23">
         <v>200</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
+      <c r="C12" s="24">
+        <v>6400</v>
+      </c>
+      <c r="D12" s="24">
+        <v>4.43997228014777</v>
+      </c>
+      <c r="E12" s="24">
+        <v>0.0643726281866623</v>
+      </c>
+      <c r="F12" s="24">
+        <v>76</v>
+      </c>
+      <c r="G12" s="24">
+        <v>16842</v>
+      </c>
+      <c r="H12" s="24">
+        <v>4.52450548097265</v>
+      </c>
+      <c r="I12" s="24">
+        <v>0.148905829011543</v>
+      </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="22">
@@ -1799,13 +1911,27 @@
       <c r="B13" s="23">
         <v>200</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
+      <c r="C13" s="24">
+        <v>12800</v>
+      </c>
+      <c r="D13" s="24">
+        <v>4.38095094845919</v>
+      </c>
+      <c r="E13" s="24">
+        <v>0.00535129649808485</v>
+      </c>
+      <c r="F13" s="24">
+        <v>96</v>
+      </c>
+      <c r="G13" s="24">
+        <v>26666</v>
+      </c>
+      <c r="H13" s="24">
+        <v>4.48844132213009</v>
+      </c>
+      <c r="I13" s="24">
+        <v>0.112841670168988</v>
+      </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="22">
@@ -1814,13 +1940,27 @@
       <c r="B14" s="23">
         <v>200</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
+      <c r="C14" s="24">
+        <v>25600</v>
+      </c>
+      <c r="D14" s="24">
+        <v>4.42351288471198</v>
+      </c>
+      <c r="E14" s="24">
+        <v>0.047913232750874</v>
+      </c>
+      <c r="F14" s="24">
+        <v>121</v>
+      </c>
+      <c r="G14" s="24">
+        <v>42314</v>
+      </c>
+      <c r="H14" s="24">
+        <v>4.45095301421708</v>
+      </c>
+      <c r="I14" s="24">
+        <v>0.0753533622559752</v>
+      </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="19"/>

</xml_diff>